<commit_message>
Added more commands (Part 2)
</commit_message>
<xml_diff>
--- a/Git & GitHub/Excel Files/Git Commands.xlsx
+++ b/Git & GitHub/Excel Files/Git Commands.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Purpose</t>
   </si>
@@ -102,6 +100,48 @@
   </si>
   <si>
     <t>git show &lt;Provide id&gt;</t>
+  </si>
+  <si>
+    <t>git branch &lt;branch Name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create new barnch </t>
+  </si>
+  <si>
+    <t>git switch &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>To switch from branch A to branch B (head will point for switched branch)</t>
+  </si>
+  <si>
+    <t>git switch -c &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>To create new barnch and direct switch to that branch</t>
+  </si>
+  <si>
+    <t>git checkout &lt;branch Name&gt;</t>
+  </si>
+  <si>
+    <t>To check if the branch is present and if present the switch to that barnch</t>
+  </si>
+  <si>
+    <t>git merge &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>To merge that changes from differnent branch to main branch (fast forward direct merge)</t>
+  </si>
+  <si>
+    <t>git branch -m &lt;old name&gt; &lt;New Name&gt;</t>
+  </si>
+  <si>
+    <t>To Change the name of the branch</t>
+  </si>
+  <si>
+    <t>git branch -d &lt;branch Name&gt;</t>
+  </si>
+  <si>
+    <t>To delete the branch (d stands for delete )</t>
   </si>
 </sst>
 </file>
@@ -133,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,11 +196,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -173,6 +233,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,32 +657,64 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>